<commit_message>
Consultas en archivo csv
Implementación de función para verificar la existencia de un usuario.
</commit_message>
<xml_diff>
--- a/password_database_ED2.xlsx
+++ b/password_database_ED2.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uninorte-my.sharepoint.com/personal/arangocarlos_uninorte_edu_co/Documents/Documentos/GitHub/hash_crypto/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_46B1146FBF16ED3FA7071F884D20C8AEE7B9CEDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B481710B-F0DC-4915-ACB1-3D7A186B06CC}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t>username</t>
   </si>
@@ -587,17 +592,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -605,29 +612,55 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5AEADC45-66AB-49B6-8A79-2498F1826D73}" name="Tabla1" displayName="Tabla1" ref="A1:C63" totalsRowShown="0">
+  <autoFilter ref="A1:C63" xr:uid="{5AEADC45-66AB-49B6-8A79-2498F1826D73}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5DDDBCB4-D6D1-4BE6-9E78-160F7984C73D}" name="username"/>
+    <tableColumn id="2" xr3:uid="{877E9E2C-3251-4DEE-9A15-7610563CE146}" name="salt"/>
+    <tableColumn id="3" xr3:uid="{47FF5859-CEB4-4074-B975-819A7D6D27C9}" name="password"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -916,19 +949,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:C63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="3" max="3" width="132.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,8 +974,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -950,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -961,7 +996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -972,7 +1007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -983,7 +1018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -994,18 +1029,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1016,7 +1051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1027,7 +1062,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1038,7 +1073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1049,7 +1084,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1060,7 +1095,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1071,7 +1106,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1082,7 +1117,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1093,7 +1128,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1104,7 +1139,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1115,7 +1150,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1126,7 +1161,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1137,7 +1172,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1148,7 +1183,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1159,7 +1194,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1170,7 +1205,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1181,7 +1216,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1192,7 +1227,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1203,7 +1238,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1214,7 +1249,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1225,7 +1260,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1236,7 +1271,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1247,7 +1282,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1258,7 +1293,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -1269,7 +1304,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -1280,7 +1315,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -1291,7 +1326,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -1302,7 +1337,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -1313,7 +1348,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -1324,7 +1359,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -1335,7 +1370,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -1346,7 +1381,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1357,7 +1392,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1368,7 +1403,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -1379,7 +1414,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -1390,7 +1425,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>126</v>
       </c>
@@ -1401,7 +1436,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>129</v>
       </c>
@@ -1412,7 +1447,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>132</v>
       </c>
@@ -1423,7 +1458,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>135</v>
       </c>
@@ -1434,7 +1469,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>138</v>
       </c>
@@ -1445,7 +1480,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -1456,7 +1491,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -1467,7 +1502,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -1478,7 +1513,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>150</v>
       </c>
@@ -1489,7 +1524,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>153</v>
       </c>
@@ -1500,7 +1535,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -1511,7 +1546,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>159</v>
       </c>
@@ -1522,7 +1557,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -1533,7 +1568,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>165</v>
       </c>
@@ -1544,7 +1579,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>168</v>
       </c>
@@ -1555,7 +1590,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>171</v>
       </c>
@@ -1566,7 +1601,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -1577,7 +1612,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -1588,7 +1623,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>180</v>
       </c>
@@ -1599,7 +1634,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>183</v>
       </c>
@@ -1610,7 +1645,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -1621,18 +1656,14 @@
         <v>188</v>
       </c>
     </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+    </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>